<commit_message>
Added false positive review as well
</commit_message>
<xml_diff>
--- a/test/false_negative.xlsx
+++ b/test/false_negative.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42188502-303B-4C20-8BE3-55273DE496F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -19,14 +20,14 @@
     <t>Phishing Email</t>
   </si>
   <si>
-    <t xml:space="preserve">Sender: WeTransfer &lt;no_reply@wetransfer.com&gt;
+    <t>Sender: WeTransfer &lt;no_reply@wetransfer.com&gt;
 Receiver: jose@monkey.org
 Date: 9 Dec 2022 15:54:58 +0000
 Subject: Jeanette.rodriguez@mcft.com sent you Product Sample and Specifications.pdf via WeTransfer
 Body: test  This transfer expires on 2022-08-25    jeanette.rodriguez@mcft.com sent you Product Sample and Specifications.pdf Â  5 items, 200 MB in total ãƒ» Expires onÂ 15 December, 2022 Product Sample and Specifications. Kindly find attached product sample, product order and company specifications Thanks &amp; Regards, Ms. Jeanette Rodriguez MCFT Trading LLC  Get your files    Â  Download link https://wetransfer.com/downloads/2ddd705c3f9194e81aad04deb30acee820220818123211/ d4c5b6a979dc7e842a4fffbb31f076cf20220818123235/46fe24 Â 5 items Product Sample 1.pdf 9 MB Product Sample 2.pdf 8 MB Sample 1 video.mp4 33 MB Sample 2 video.mp4 109 MB Specifications.pdf 41 MB To make sure our emails arrive, please add noreply@wetransfer.com  to your contacts. About WeTransfer Â Â ãƒ»Â Â  Help Â Â ãƒ»Â Â  Legal Â Â ãƒ»Â Â  Report this transfer as spam</t>
   </si>
   <si>
-    <t xml:space="preserve">The student may have wrongly identified this email as legitimate because it appears to be from WeTransfer, a legitimate file-sharing service, and includes details about a file being sent, which can create a sense of urgency or curiosity to download the attachment.
+    <t>The student may have wrongly identified this email as legitimate because it appears to be from WeTransfer, a legitimate file-sharing service, and includes details about a file being sent, which can create a sense of urgency or curiosity to download the attachment.
 However, there are several features of this email that indicate it is actually a malicious phishing attempt:
 1. **Suspicious Sender Address**: While the sender name appears as WeTransfer, the actual email address is 'no_reply@wetransfer.com'. Phishers often spoof email addresses to make them look legitimate, but a careful examination of the email address can reveal the discrepancy.
 2. **Urgency**: The email creates a sense of urgency by stating that the transfer expires soon and urging the recipient to download the files. Phishing emails often use urgency to prompt recipients to act before thinking critically.
@@ -38,7 +39,7 @@
 By considering these red flags and conducting a closer inspection of the email, it becomes evident that it is a phishing attempt rather than a legitimate communication from WeTransfer.</t>
   </si>
   <si>
-    <t xml:space="preserve">Sender: "Help Center" &lt;55133482420802311482@help.nuren.co&gt;
+    <t>Sender: "Help Center" &lt;55133482420802311482@help.nuren.co&gt;
 Receiver: jose@monkey.org
 Date: Fri, 21 Oct 2022 13:32:25 +0000
 Subject: We're having some trouble with your current billing information 
@@ -50,7 +51,7 @@
  UPDATE YOUR DETAILS Â Â Â Â Â Â Â Â Â Â Â  Â Â  NETFLIX Dear Customer, We're having some trouble with your current billing information. We'll try again, but in the meantime you may want to update your payment details. Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â Â  UPDATE YOUR DETAILS</t>
   </si>
   <si>
-    <t xml:space="preserve">The student may have wrongly identified this email as legitimate due to the following reasons:
+    <t>The student may have wrongly identified this email as legitimate due to the following reasons:
 1. **Display Name Mismatch**: The sender's email address is suspicious. Legitimate emails from a company like Netflix would usually come from an email address containing the company's name (e.g., support@netflix.com). In this case, the sender's email address is a random string of numbers followed by '@help.nuren.co', which is not a standard Netflix domain.
 2. **Urgency and Threat**: Phishing emails often create a sense of urgency or threat to prompt the recipient to act quickly without thinking. In this email, the threat of having trouble with billing information and the suggestion to update payment details immediately can induce panic and lead the recipient to overlook other red flags.
 3. **Poor Grammar and Formatting**: Legitimate companies typically have professional communication with correct grammar and formatting. In this email, there are multiple instances of strange characters (e.g., 'Â ') and repetitive text, which are indicators of a phishing attempt.
@@ -59,14 +60,14 @@
 In conclusion, the student overlooked these classic signs of a phishing email, including the suspicious sender's address, urgency, poor grammar, generic greeting, and the presence of potentially malicious links. Training should emphasize these characteristics to help students better recognize and avoid falling victim to phishing attacks.</t>
   </si>
   <si>
-    <t xml:space="preserve">Sender: "monkey.org Mail Center" &lt;jose@genfiak.host&gt;
+    <t>Sender: "monkey.org Mail Center" &lt;jose@genfiak.host&gt;
 Receiver: jose@monkey.org
 Date: 30 Nov 2022 02:54:50 -0800
 Subject: 7 unread encrypted emails received
 Body: domain555.html You haveÂ 7 secure messages in the server Date: 11/30/2022 2:54:50 a.m. Account:jose@monkey.org  Â 	   You receivedÂ 14 important encrypted messages to your email jose@monkey.org. Follow this link to read your encrypted message.Â Secured messages cannot be viewed directly in your mailbox.Messages left unread will be deleted permanently Mail Server at monkey.org</t>
   </si>
   <si>
-    <t xml:space="preserve">At first glance, this email may appear to be legitimate due to the presence of some characteristics typically found in phishing emails. Here are some features that have been overlooked by the student, ultimately leading to the erroneous identification of the email as legitimate:
+    <t>At first glance, this email may appear to be legitimate due to the presence of some characteristics typically found in phishing emails. Here are some features that have been overlooked by the student, ultimately leading to the erroneous identification of the email as legitimate:
 1. **Unsolicited email**: Phishing emails are often unsolicited, meaning the recipient did not request or expect to receive the email. In this case, the email claims that the recipient has unread encrypted messages without any prior communication or context.
 2. **Urgency**: Phishing emails often create a sense of urgency to prompt quick action from the recipient. In this email, the statement "Messages left unread will be deleted permanently" creates a sense of urgency to click the provided link without taking the time to verify the authenticity of the email.
 3. **Mismatched sender and domain**: While the sender name appears as "monkey.org Mail Center," the actual email address is from a different domain - "jose@genfiak.host." This mismatch between the sender's displayed name and the email address is a common tactic used in phishing emails to deceive recipients.
@@ -75,14 +76,14 @@
 By paying attention to these overlooked features and behaviors commonly found in phishing emails, the student could have correctly identified this email as malicious rather than legitimate.</t>
   </si>
   <si>
-    <t xml:space="preserve">Sender: "emailadmin@monkey.org" &lt;monkey.org-5901617@koonja-copyright.com&gt;
+    <t>Sender: "emailadmin@monkey.org" &lt;monkey.org-5901617@koonja-copyright.com&gt;
 Receiver: &lt;jose@monkey.org&gt;
 Date: Tue, 18 Oct 2022 22:58:00 -0700
 Subject: - Queued Message Notification -  id:2vFioVYa
 Body: Queued Messages Notification Valued jose, Your messages are queued up and pending delivery as of Tuesday, October 18, 2022. Tap below and sign-in to verify your mailbox so that the functions of the mail can be restored. Verify Thank You monkey.org Webmail Support   Queued Messages NotificationValued jose,Your messages are queued up and pending delivery as of Tuesday, October 18, 2022. Tap below and sign-in to verify your mailbox so that the functions of the mail can be restored. VerifyThank Youmonkey.org Webmail Support</t>
   </si>
   <si>
-    <t xml:space="preserve">The student may have wrongly identified this email as legitimate because of the following reasons:
+    <t>The student may have wrongly identified this email as legitimate because of the following reasons:
 1. **Display Name vs. Email Address:** The sender's display name appears as "emailadmin@monkey.org," which might trick the receiver into thinking it is from the legitimate domain "monkey.org". However, the actual email address is "&lt;monkey.org-5901617@koonja-copyright.com&gt;", which is suspicious and not related to the claimed sender domain.
 2. **Urgency and Fear Tactics:** The email creates a sense of urgency by claiming that the recipient's messages are queued up and pending delivery. Phishing emails often use fear tactics to prompt recipients to take immediate action without thinking critically.
 3. **Phishing Links:** The email contains a link that asks the recipient to sign in to verify their mailbox. This is a common tactic used in phishing emails to steal login credentials. Hovering over the link (without clicking) would likely reveal that it doesn't lead to the claimed website.
@@ -92,14 +93,14 @@
 In conclusion, the student may have overlooked these typical phishing email characteristics, including suspicious sender details, urgency, phishing links, generic greetings, grammar errors, and potential malicious attachments or links. Understanding these red flags can help in correctly identifying such emails as malicious phishing attempts.</t>
   </si>
   <si>
-    <t xml:space="preserve">Sender: Email administrator &lt;mikem@danawallboard.com&gt;
+    <t>Sender: Email administrator &lt;mikem@danawallboard.com&gt;
 Receiver: jose@monkey.org
 Date: Mon, 07 Nov 2022 17:17:15 +0000 (UTC)
 Subject: jose@monkey.org:Password Expiration Notification
 Body: Hi jose@monkey.org  Password for (jose@monkey.org) expires today  Monday 7,Nov.   Keep My Same Password   Â  Hi jose@monkey.org Password forÂ (jose@monkey.org)Â expires today Monday 7,Nov. Keep My Same Password</t>
   </si>
   <si>
-    <t xml:space="preserve">The student may have wrongly identified this email as legitimate due to several reasons:
+    <t>The student may have wrongly identified this email as legitimate due to several reasons:
 1. **Spelling and Grammar Errors:** The email contains multiple spelling and grammar errors such as "Keep My Same Password Â " and "Password forÂ (jose@monkey.org)Â expires today Monday 7,Nov." Legitimate organizations usually have proper proofreading processes in place, so the presence of such errors is a red flag for phishing emails.
 2. **Urgency and Threats:** The email creates a sense of urgency by stating that the password expires on the same day it was sent. Phishing emails often use urgency or threats to push the recipient into taking immediate action without thinking critically.
 3. **Mismatched Email Contents:** The subject line mentions "Password Expiration Notification," but the content of the email does not provide a clear reason or specific instructions on what the recipient needs to do. This mismatch is often a sign of a phishing attempt, where scammers use generic templates to target a wide range of users.
@@ -110,7 +111,7 @@
 By paying attention to these overlooked features, the student can learn to better identify phishing emails and avoid falling victim to cyber scams.</t>
   </si>
   <si>
-    <t xml:space="preserve">Sender: Help Center &lt;help_center_7360403570@em8042.wilms-ch.org&gt;
+    <t>Sender: Help Center &lt;help_center_7360403570@em8042.wilms-ch.org&gt;
 Receiver: jose@monkey.org
 Date: Mon, 21 Nov 2022 08:37:02 +0000 (UTC)
 Subject: We're having some trouble with your current billing information
@@ -124,7 +125,7 @@
 Netflix billing team. Â Â Â Â Â Â Â Â  NETFLIX Â  Dear Customer, We're having some trouble with your current billing information. We'll try again, but in the meantime you may want to update your payment details. click on the button bellow to update your account now. &gt;&gt;Update my Account Â  Thank you for choosing Netflix. Netflix billing team.</t>
   </si>
   <si>
-    <t xml:space="preserve">The student may have wrongly identified this email as legitimate due to the following reasons:
+    <t>The student may have wrongly identified this email as legitimate due to the following reasons:
 1. **Sender Name Mismatch**: While the sender name appears as "Help Center," the actual email address it is sent from is suspicious and does not match a typical Help Center domain. The email is sent from help_center_7360403570@em8042.wilms-ch.org, which is not a legitimate Netflix domain.
 2. **Urgency and Threats**: Phishing emails often create a sense of urgency or threat to prompt the recipient to act quickly without thinking. In this email, the threat of "trouble with your billing information" and the urgent request to update payment details by clicking a link can be tactics used to manipulate the recipient.
 3. **Generic Greeting**: The email starts with "Dear Customer" instead of addressing the recipient by their name. Legitimate companies usually personalize emails by including the recipient's name.
@@ -133,7 +134,7 @@
 In conclusion, the student overlooked key elements that are often present in phishing emails such as suspicious sender addresses, urgent and threatening language, lack of personalization, poor grammar and formatting, and requests for sensitive information or actions. These are red flags that indicate the email is likely a phishing attempt rather than a legitimate communication from Netflix.</t>
   </si>
   <si>
-    <t xml:space="preserve">Sender: "Help Center" &lt;info@vccedge.com&gt;
+    <t>Sender: "Help Center" &lt;info@vccedge.com&gt;
 Receiver: jose@monkey.org
 Date: Sat, 26 Nov 2022 11:12:46 +0000
 Subject: Your account is on hold.
@@ -148,7 +149,7 @@
  Â  Your account is on hold.  Payment details update required.  Hello,  We're having some trouble with your current billing information. We'll try again, but in the meantime you need to update your payment details.  UPDATE YOUR ACCOUNT  Need help? We areÂ available if you need it. Visit the Help Center or contact us .  -Your friends at Netflix</t>
   </si>
   <si>
-    <t xml:space="preserve">The student may have wrongly identified this email as legitimate because it appears to be from a familiar company, Netflix, and the email formatting looks professional. However, there are several features of this email that indicate it is actually a malicious phishing attempt:
+    <t>The student may have wrongly identified this email as legitimate because it appears to be from a familiar company, Netflix, and the email formatting looks professional. However, there are several features of this email that indicate it is actually a malicious phishing attempt:
 1. **Urgency and Threats**: The email creates a sense of urgency by claiming that the recipient's account is on hold and payment details need to be updated immediately. Phishing emails often use this tactic to pressure recipients into taking immediate action without thinking it through.
 2. **Mismatched Sender Address**: While the sender appears to be "Help Center" from info@vccedge.com, the content of the email is related to Netflix. This inconsistency is a red flag in phishing emails. Cybercriminals often use spoofed or fake email addresses to trick recipients.
 3. **Generic Greeting**: The email starts with a generic greeting "Hello" instead of addressing the recipient by name. Legitimate companies usually use personalized greetings that include the recipient's name.
@@ -158,7 +159,7 @@
 By overlooking these key features of phishing emails, the student incorrectly identified this phishing email as legitimate. It's important to always remain cautious and scrutinize such emails carefully before taking any action to avoid falling victim to phishing attacks.</t>
   </si>
   <si>
-    <t xml:space="preserve">Sender: Binance &lt;support@hale.itsahappyclient.com&gt;
+    <t>Sender: Binance &lt;support@hale.itsahappyclient.com&gt;
 Receiver: jose@monkey.org
 Date: Tue, 08 Nov 2022 22:43:01 +0000 (UTC)
 Subject: [Binance] Login Attempted from New IP address 285.128.9.147 -
@@ -166,7 +167,7 @@
 Body: Did You Login From a New Device or Location? We noticed your Binance accountÂ jose@monkey.orgÂ was accessed from a new IP address.Â We have suspended your account, Kindly visit the button belowÂ to re-activateWhenÂ  : 2022-11-08 12:47:58(UTC)IP AddressÂ : 285.128.9.147 Visit Your Account.Â This is an automated message, please do not reply.Â  Stay connected! Â  Â  Â  Â  Â  Â  To stay secure, setup your phishing codeÂ  hereÂ  Risk warning:Â Cryptocurrency trading is subject to high market risk. Binance will make the best efforts to choose high-quality coins, but will not be responsible for your trading losses. Please trade with caution. Kindly note:Â Please be aware of phishing sites and always make sure you are visiting the officialÂ Binance.comÂ website when entering sensitive data. Â© 2017 - 2022Â  Binance.com, All Rights Reserved. Did You Login From a New Device or Location? We noticed your Binance accountÂ jose@monkey.orgÂ was accessed from a new IP address.Â We have suspended your account, Kindly visit the button belowÂ to re-activateWhenÂ  : 2022-11-08 12:47:58(UTC)IP AddressÂ : 285.128.9.147 Visit Your Account.Â This is an automated message, please do not reply.Â  Stay connected! Â  Â  Â  Â  Â  Â  To stay secure, setup your phishing codeÂ  hereÂ  Risk warning:Â Cryptocurrency trading is subject to high market risk. Binance will make the best efforts to choose high-quality coins, but will not be responsible for your trading losses. Please trade with caution. Kindly note:Â Please be aware of phishing sites and always make sure you are visiting the officialÂ Binance.comÂ website when entering sensitive data. Â© 2017 - 2022Â  Binance.com, All Rights Reserved.</t>
   </si>
   <si>
-    <t xml:space="preserve">The student may have wrongly identified this email as legitimate due to a few reasons:
+    <t>The student may have wrongly identified this email as legitimate due to a few reasons:
 1. **Sender Name**: The email appears to be sent from "Binance." However, upon closer inspection, the actual email address is "support@hale.itsahappyclient.com," which is not a legitimate Binance domain. Phishing emails often spoof the sender's name to appear as a trusted entity while actually coming from a different, malicious source.
 2. **Urgency**: The email creates a sense of urgency by stating that the recipient's account has been accessed from a new IP address and that their account has been suspended. Phishing emails often use urgency and fear tactics to prompt quick actions without giving the recipient much time to think logically.
 3. **Suspicious Links**: The email contains a link for the recipient to click to "visit your account" and supposedly reactivate it. However, this link could lead to a phishing website designed to steal the recipient's login credentials or other sensitive information. Always hover over links in emails to see the actual URL before clicking on them.
@@ -176,14 +177,14 @@
 In conclusion, the student may have overlooked these key phishing indicators, such as the mismatched sender email address, urgency, suspicious links, grammatical errors, unusual requests, and lack of personalization, leading them to mistakenly identify this malicious email as legitimate.</t>
   </si>
   <si>
-    <t xml:space="preserve">Sender: Server Admin monkey.org &lt;kapcsolat@emus.hu&gt;
+    <t>Sender: Server Admin monkey.org &lt;kapcsolat@emus.hu&gt;
 Receiver: jose@monkey.org
 Date: 2 Nov 2022 14:57:46 +0100
 Subject: monkey.org Server - Password Expired
 Body: monkey.org Server - Password ExpiredÂ  Â  The password to your Â mailboxÂ jose@monkey.orgÂ has expired. System will log you out and generate a new password exactly at 24 hours from  3 Nov 2022. .Â Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â Â  Â  Â You can continue using your current password. Use the button below to keep using current password.Â  Â    Keep Current PasswordÂ  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â  Â Â Â  Â  Â  Â  Â  Â  Â  Â  Email is generated by monkey.org Email Server forÂ jose@monkey.org</t>
   </si>
   <si>
-    <t xml:space="preserve">The student may have wrongly identified this email as legitimate due to several reasons. Here are some features of a phishing email that have been overlooked by the student:
+    <t>The student may have wrongly identified this email as legitimate due to several reasons. Here are some features of a phishing email that have been overlooked by the student:
 1. **Unusual Sender Email Address**: The sender's email address is kapcsolat@emus.hu, which is not a typical address for a legitimate server admin of monkey.org. Phishing emails often use spoofed or slightly altered email addresses to deceive recipients.
 2. **Urgency and Threat**: Phishing emails often create a sense of urgency or fear to prompt the recipient to take immediate action without thinking. In this case, the email states that the password has expired and will be changed automatically if not acted upon promptly. This pressure tactic is commonly used in phishing emails.
 3. **Incorrect Grammar and Spelling**: The email contains grammar errors such as "Â mailboxÂ jose@monkey.orgÂ has expired" and extra characters like "Â " which are common in phishing emails. Legitimate organizations usually have proper proofreading in place for their official emails.
@@ -196,14 +197,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -226,8 +227,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,93 +511,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="255.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="14.4" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="14.4" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="14.4" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>